<commit_message>
Update accomodation text, added visby börs and donners
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/royfr474/github/raukr-2026/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56219A2C-D162-F445-B35E-A2672FE070EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F858A22C-9836-4C4F-A069-4CE03E5452FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3280" yWindow="6240" windowWidth="22560" windowHeight="16380" xr2:uid="{5F8B95CE-8379-E541-8BD7-284A0F505EB1}"/>
+    <workbookView xWindow="800" yWindow="5220" windowWidth="22560" windowHeight="16380" xr2:uid="{5F8B95CE-8379-E541-8BD7-284A0F505EB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="info" localSheetId="0">Sheet1!$A$1:$F$11</definedName>
+    <definedName name="info" localSheetId="0">Sheet1!$A$1:$F$13</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="58">
   <si>
     <t>marker_icon</t>
   </si>
@@ -213,6 +213,24 @@
   </si>
   <si>
     <t>Strandgatan 34, 621 56 Visby (8 min walk, 2 min bike)</t>
+  </si>
+  <si>
+    <t>Strandgatan 10, 621 56 Visby, 290m (4 min walk)</t>
+  </si>
+  <si>
+    <t>Visby Börs</t>
+  </si>
+  <si>
+    <t>https://visbybors.se/</t>
+  </si>
+  <si>
+    <t>https://donnershotell.se/</t>
+  </si>
+  <si>
+    <t>Donners Hotell</t>
+  </si>
+  <si>
+    <t>Donnersgatan 6, 621 57 Visby, 290m (4 min walk)</t>
   </si>
 </sst>
 </file>
@@ -584,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C682103A-4E94-8940-91C1-6B6AF5A5418B}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="F19" sqref="F19:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -655,19 +673,19 @@
         <v>9</v>
       </c>
       <c r="C3" s="1">
-        <v>57.6418222910998</v>
+        <v>57.639545750572502</v>
       </c>
       <c r="D3" s="1">
-        <v>18.292492482687901</v>
+        <v>18.292112396306099</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -678,19 +696,19 @@
         <v>9</v>
       </c>
       <c r="C4" s="1">
-        <v>57.638648934832403</v>
+        <v>57.638815439200499</v>
       </c>
       <c r="D4" s="1">
-        <v>18.2909058341587</v>
+        <v>18.291531757191901</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -701,19 +719,19 @@
         <v>9</v>
       </c>
       <c r="C5" s="1">
-        <v>57.6431496715119</v>
+        <v>57.6418222910998</v>
       </c>
       <c r="D5" s="1">
-        <v>18.295927671047401</v>
+        <v>18.292492482687901</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -724,19 +742,19 @@
         <v>9</v>
       </c>
       <c r="C6" s="1">
-        <v>57.632070532262503</v>
+        <v>57.638648934832403</v>
       </c>
       <c r="D6" s="1">
-        <v>18.28036866919</v>
+        <v>18.2909058341587</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -747,19 +765,19 @@
         <v>9</v>
       </c>
       <c r="C7" s="1">
-        <v>57.636482062595299</v>
+        <v>57.6431496715119</v>
       </c>
       <c r="D7" s="1">
-        <v>18.2894577665854</v>
+        <v>18.295927671047401</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -770,19 +788,19 @@
         <v>9</v>
       </c>
       <c r="C8" s="1">
-        <v>57.625870354994802</v>
+        <v>57.632070532262503</v>
       </c>
       <c r="D8" s="1">
-        <v>18.2820583121987</v>
+        <v>18.28036866919</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -793,19 +811,19 @@
         <v>9</v>
       </c>
       <c r="C9" s="1">
-        <v>57.655401082862802</v>
+        <v>57.636482062595299</v>
       </c>
       <c r="D9" s="1">
-        <v>18.307905867869199</v>
+        <v>18.2894577665854</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -833,86 +851,134 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1">
-        <v>57.634235891617003</v>
+        <v>57.655401082862802</v>
       </c>
       <c r="D11" s="1">
-        <v>18.281245993358699</v>
+        <v>18.307905867869199</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="C12" s="1">
-        <v>57.660792685490399</v>
+        <v>57.625870354994802</v>
       </c>
       <c r="D12" s="1">
-        <v>18.33859496282</v>
+        <v>18.2820583121987</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="1">
+        <v>57.634235891617003</v>
+      </c>
+      <c r="D13" s="1">
+        <v>18.281245993358699</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="1">
+        <v>57.660792685490399</v>
+      </c>
+      <c r="D14" s="1">
+        <v>18.33859496282</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C15" s="1">
         <v>57.641785617708997</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D15" s="1">
         <v>18.296064226832399</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G10" r:id="rId1" xr:uid="{76E7C569-DDDB-3B41-9B07-B6521B3D1063}"/>
-    <hyperlink ref="G7" r:id="rId2" xr:uid="{A9CA159D-1489-D148-BBAB-AD4975BC4631}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{EF76D4CB-5E4C-D948-8B7F-2FA544401467}"/>
+    <hyperlink ref="G9" r:id="rId2" xr:uid="{A9CA159D-1489-D148-BBAB-AD4975BC4631}"/>
+    <hyperlink ref="G6" r:id="rId3" xr:uid="{EF76D4CB-5E4C-D948-8B7F-2FA544401467}"/>
     <hyperlink ref="G2" r:id="rId4" xr:uid="{E13D6187-13EC-7E4F-ADC2-1F164AB0E785}"/>
-    <hyperlink ref="G11" r:id="rId5" xr:uid="{24169AD6-3270-7546-B069-9815CD90E4EE}"/>
-    <hyperlink ref="G12" r:id="rId6" xr:uid="{9AED9BB7-3026-FE42-A6FD-3C141EDDA6CF}"/>
-    <hyperlink ref="G8" r:id="rId7" xr:uid="{4705B889-D875-9940-ABAB-39B15F6453CC}"/>
-    <hyperlink ref="G9" r:id="rId8" xr:uid="{11650BD3-7118-BE4D-A3EA-DF5D877777C7}"/>
-    <hyperlink ref="G6" r:id="rId9" xr:uid="{CC457E57-09F2-214B-9915-8076F571C766}"/>
-    <hyperlink ref="G5" r:id="rId10" xr:uid="{8778F495-0377-894C-B29F-9C59832EC0F5}"/>
-    <hyperlink ref="G3" r:id="rId11" xr:uid="{C6BFCFE6-6075-884C-BE02-1DDA5B096A8F}"/>
+    <hyperlink ref="G13" r:id="rId5" xr:uid="{24169AD6-3270-7546-B069-9815CD90E4EE}"/>
+    <hyperlink ref="G14" r:id="rId6" xr:uid="{9AED9BB7-3026-FE42-A6FD-3C141EDDA6CF}"/>
+    <hyperlink ref="G12" r:id="rId7" xr:uid="{4705B889-D875-9940-ABAB-39B15F6453CC}"/>
+    <hyperlink ref="G11" r:id="rId8" xr:uid="{11650BD3-7118-BE4D-A3EA-DF5D877777C7}"/>
+    <hyperlink ref="G8" r:id="rId9" xr:uid="{CC457E57-09F2-214B-9915-8076F571C766}"/>
+    <hyperlink ref="G7" r:id="rId10" xr:uid="{8778F495-0377-894C-B29F-9C59832EC0F5}"/>
+    <hyperlink ref="G5" r:id="rId11" xr:uid="{C6BFCFE6-6075-884C-BE02-1DDA5B096A8F}"/>
+    <hyperlink ref="G3" r:id="rId12" xr:uid="{4FC7EA8A-F842-E746-9F1A-59587BBACB32}"/>
+    <hyperlink ref="G4" r:id="rId13" xr:uid="{D6B091B9-EB05-E446-B3B2-73D9DEEE2D02}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>